<commit_message>
update max date 16feb
</commit_message>
<xml_diff>
--- a/database/KICT Backup DB/Insert_Query.xlsx
+++ b/database/KICT Backup DB/Insert_Query.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Azmi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/kict-dev/database/KICT Backup DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAB8077-B13E-7441-9D1F-EF004CA4CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD951025-E654-4746-8B26-32B90102EC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="3" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
+    <workbookView xWindow="2120" yWindow="1500" windowWidth="23260" windowHeight="12460" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="301">
   <si>
     <t>staff_id</t>
   </si>
@@ -699,18 +699,12 @@
     <t>program_name</t>
   </si>
   <si>
-    <t>CITA</t>
-  </si>
-  <si>
     <t>INFO 7011</t>
   </si>
   <si>
     <t>Islamic Worldview on ICT and Society</t>
   </si>
   <si>
-    <t>DIS</t>
-  </si>
-  <si>
     <t>INFO 7901</t>
   </si>
   <si>
@@ -912,22 +906,43 @@
     <t>LISC 7020</t>
   </si>
   <si>
-    <t>DLIS</t>
-  </si>
-  <si>
-    <t>Master in Protective Security Management (MPSM)</t>
-  </si>
-  <si>
-    <t>Master in Business Intelligence And Analytic (MBIA)</t>
-  </si>
-  <si>
     <t>Master of Library and Information Science</t>
   </si>
   <si>
     <t>Master of Information Technology</t>
   </si>
   <si>
-    <t>Doctor of Philosophy (Library and Information Science)</t>
+    <t>MPSM</t>
+  </si>
+  <si>
+    <t>MBIA</t>
+  </si>
+  <si>
+    <t>MLIB</t>
+  </si>
+  <si>
+    <t>MITEC</t>
+  </si>
+  <si>
+    <t>Master in Protective Security Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master in Business Intelligence And Analytic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSLINA OTHMAN </t>
+  </si>
+  <si>
+    <t>ROOSFA HASHIM</t>
+  </si>
+  <si>
+    <t>SHARIFAH NUR AMIRAH SARIF ABDULLAH</t>
+  </si>
+  <si>
+    <t>NOR SAADAH MD. NOR</t>
+  </si>
+  <si>
+    <t>NUR LEYNI NILAM PUTRI JUNURHAM</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1035,13 +1050,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1356,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050F0502-707F-E94C-BAD9-F21BCE0BBD9A}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1375,7 @@
     <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="4" width="14.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2571,7 +2579,7 @@
         <v>5</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E71" si="1">"INSERT INTO staff VALUES('"&amp;A67&amp;"','"&amp;B67&amp;"', "&amp;C67&amp;", "&amp;D67&amp;");"</f>
+        <f t="shared" ref="E67:E76" si="1">"INSERT INTO staff VALUES('"&amp;A67&amp;"','"&amp;B67&amp;"', "&amp;C67&amp;", "&amp;D67&amp;");"</f>
         <v>INSERT INTO staff VALUES('9954','TAKUMI SASE', null, null);</v>
       </c>
     </row>
@@ -2645,6 +2653,96 @@
       <c r="E71" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO staff VALUES('10722','ABDUL WAHAB BIN ABDUL RAHMAN', null, null);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>1675</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('1675','ROSLINA OTHMAN ', null, null);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>7684</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('7684','ROOSFA HASHIM', null, null);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>8227</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('8227','SHARIFAH NUR AMIRAH SARIF ABDULLAH', null, null);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>9019</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('9019','NOR SAADAH MD. NOR', null, null);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>9041</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('9041','NUR LEYNI NILAM PUTRI JUNURHAM', null, null);</v>
       </c>
     </row>
   </sheetData>
@@ -4106,7 +4204,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4139,11 +4237,11 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
         <v>220</v>
       </c>
-      <c r="B2" t="s">
-        <v>221</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4151,19 +4249,19 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>222</v>
+        <v>293</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F37" si="0">"INSERT INTO courses VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"', "&amp;C2&amp;", "&amp;D2&amp;", '"&amp;E2&amp;"');"</f>
-        <v>INSERT INTO courses VALUES('INFO 7011','Islamic Worldview on ICT and Society', null, null, 'DIS');</v>
+        <f>"INSERT INTO courses VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"', '"&amp;E2&amp;"');"</f>
+        <v>INSERT INTO courses VALUES('INFO 7011','Islamic Worldview on ICT and Society', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -4171,20 +4269,20 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>222</v>
+      <c r="E3" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7901','ICT Research Methods', null, null, 'DIS');</v>
+        <f t="shared" ref="F3:F37" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"', '"&amp;E3&amp;"');"</f>
+        <v>INSERT INTO courses VALUES('INFO 7901','ICT Research Methods', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -4192,20 +4290,20 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>222</v>
+      <c r="E4" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7131','IT Project &amp; Change Management', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7131','IT Project &amp; Change Management', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -4213,20 +4311,20 @@
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>222</v>
+      <c r="E5" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7151','IT Strategy &amp; Governance', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7151','IT Strategy &amp; Governance', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -4234,20 +4332,20 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>222</v>
+      <c r="E6" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7145','Methodologies for System Development', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7145','Methodologies for System Development', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -4255,20 +4353,20 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>222</v>
+      <c r="E7" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7991','Computing Project', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7991','Computing Project', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -4276,20 +4374,20 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>222</v>
+      <c r="E8" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7115','Advanced Data Management', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7115','Advanced Data Management', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -4297,20 +4395,20 @@
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>222</v>
+      <c r="E9" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7125','Business Data Communications &amp; Networking', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7125','Business Data Communications &amp; Networking', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -4318,20 +4416,20 @@
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>222</v>
+      <c r="E10" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7165','Advanced Enterprise Integration', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7165','Advanced Enterprise Integration', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -4339,20 +4437,20 @@
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>222</v>
+      <c r="E11" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7211','Knowledge Management Principles &amp; Practices', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7211','Knowledge Management Principles &amp; Practices', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -4360,20 +4458,20 @@
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>222</v>
+      <c r="E12" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7221','Advanced E-Commerce', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7221','Advanced E-Commerce', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -4381,20 +4479,20 @@
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>222</v>
+      <c r="E13" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7231','Cybersecurity Challenges, Policy &amp; Strategy', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7231','Cybersecurity Challenges, Policy &amp; Strategy', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -4402,20 +4500,20 @@
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>222</v>
+      <c r="E14" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7251','Mobile Communications &amp; Networks', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7251','Mobile Communications &amp; Networks', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -4423,20 +4521,20 @@
       <c r="D15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>222</v>
+      <c r="E15" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7261','IT Professional Practices', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7261','IT Professional Practices', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -4444,20 +4542,20 @@
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>222</v>
+      <c r="E16" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7271','Human Computer Interaction &amp; Design', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7271','Human Computer Interaction &amp; Design', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -4465,20 +4563,20 @@
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>222</v>
+      <c r="E17" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('NFO 7992','IT Research Proposal', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('NFO 7992','IT Research Proposal', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -4486,20 +4584,20 @@
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>222</v>
+      <c r="E18" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 7993','IT Dissertation', null, null, 'DIS');</v>
+        <v>INSERT INTO courses VALUES('INFO 7993','IT Dissertation', 'null', 'null', 'MITEC');</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -4508,19 +4606,19 @@
         <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CITA 7011 ','Islamic Worldview on IT and Society ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CITA 7011 ','Islamic Worldview on IT and Society ', 'null', 'null', 'MBIA');</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -4529,19 +4627,19 @@
         <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CBIA 7101 ','Big Data Across Verticals and Domains ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CBIA 7101 ','Big Data Across Verticals and Domains ', 'null', 'null', 'MBIA');</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -4550,19 +4648,19 @@
         <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CBIA 7102 ','Data Quality ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CBIA 7102 ','Data Quality ', 'null', 'null', 'MBIA');</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -4571,19 +4669,19 @@
         <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CBIA 7202 ','Unstructured Data Analytics ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CBIA 7202 ','Unstructured Data Analytics ', 'null', 'null', 'MBIA');</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -4592,19 +4690,19 @@
         <v>5</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CBIA 7301 ','Datathon and Bootcamp ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CBIA 7301 ','Datathon and Bootcamp ', 'null', 'null', 'MBIA');</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -4613,19 +4711,19 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CCSM 7301 ','Risk Management ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CCSM 7301 ','Risk Management ', 'null', 'null', 'MPSM');</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -4634,19 +4732,19 @@
         <v>5</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CCSM 7101 ','Business Continuity &amp; Disaster Recovery ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CCSM 7101 ','Business Continuity &amp; Disaster Recovery ', 'null', 'null', 'MPSM');</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -4655,19 +4753,19 @@
         <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CCSM 7102 ','Physical Protective Security ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CCSM 7102 ','Physical Protective Security ', 'null', 'null', 'MPSM');</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B27" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -4676,19 +4774,19 @@
         <v>5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CCSM 7998 ','Dissertation ', null, null, 'CITA');</v>
+        <v>INSERT INTO courses VALUES('CCSM 7998 ','Dissertation ', 'null', 'null', 'MPSM');</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -4697,19 +4795,19 @@
         <v>5</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7070','Management of Information Institutions', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7070','Management of Information Institutions', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -4718,19 +4816,19 @@
         <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7120','Information Analysis and Organization I', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7120','Information Analysis and Organization I', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -4739,19 +4837,19 @@
         <v>5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="F30:F31" si="1">"INSERT INTO courses VALUES('"&amp;A30&amp;"','"&amp;B30&amp;"', "&amp;C30&amp;", "&amp;D30&amp;", '"&amp;E30&amp;"');"</f>
-        <v>INSERT INTO courses VALUES('LISC 7071','Management of Information Institutions', null, null, 'DLIS');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('LISC 7071','Management of Information Institutions', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B31" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -4760,19 +4858,19 @@
         <v>5</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO courses VALUES('LISC 7020','Information Analysis and Organization I', null, null, 'DLIS');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('LISC 7020','Information Analysis and Organization I', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -4781,19 +4879,19 @@
         <v>5</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7121','Information Analysis and Organization II', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7121','Information Analysis and Organization II', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -4802,19 +4900,19 @@
         <v>5</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7420','Application of Information Technology in Library', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7420','Application of Information Technology in Library', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -4823,19 +4921,19 @@
         <v>5</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" ref="F34" si="2">"INSERT INTO courses VALUES('"&amp;A34&amp;"','"&amp;B34&amp;"', "&amp;C34&amp;", "&amp;D34&amp;", '"&amp;E34&amp;"');"</f>
-        <v>INSERT INTO courses VALUES('LISC 7421','Application of Information Technology in Library', null, null, 'DLIS');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('LISC 7421','Application of Information Technology in Library', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B35" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -4844,19 +4942,19 @@
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7430','Digital Library', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7430','Digital Library', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -4865,19 +4963,19 @@
         <v>5</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7135','Records and Archives Management', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7135','Records and Archives Management', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -4886,11 +4984,11 @@
         <v>5</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('LISC 7440','Information Processing and Database Development', null, null, 'DLIS');</v>
+        <v>INSERT INTO courses VALUES('LISC 7440','Information Processing and Database Development', 'null', 'null', 'MLIB');</v>
       </c>
     </row>
   </sheetData>
@@ -4901,16 +4999,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B4B34A-38F9-E84B-918E-E2FD74ABAF9E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="46.1640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="46.1640625" customWidth="1"/>
     <col min="3" max="4" width="14.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="97.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4934,10 +5032,10 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -4946,16 +5044,16 @@
         <v>5</v>
       </c>
       <c r="E2" t="str">
-        <f>"INSERT INTO p_g_programs VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"', "&amp;C2&amp;", "&amp;D2&amp;"');"</f>
-        <v>INSERT INTO p_g_programs VALUES('CITA','Master in Protective Security Management (MPSM)', null, null');</v>
+        <f>"INSERT INTO p_g_programs VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"',' "&amp;C2&amp;"',' "&amp;D2&amp;"');"</f>
+        <v>INSERT INTO p_g_programs VALUES('MPSM','Master in Protective Security Management',' null',' null');</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>295</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -4964,16 +5062,16 @@
         <v>5</v>
       </c>
       <c r="E3" t="str">
-        <f>"INSERT INTO p_g_programs VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;"');"</f>
-        <v>INSERT INTO p_g_programs VALUES('CITA','Master in Business Intelligence And Analytic (MBIA)', null, null');</v>
+        <f t="shared" ref="E3:E5" si="0">"INSERT INTO p_g_programs VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"',' "&amp;C3&amp;"',' "&amp;D3&amp;"');"</f>
+        <v>INSERT INTO p_g_programs VALUES('MBIA','Master in Business Intelligence And Analytic ',' null',' null');</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>289</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -4982,16 +5080,16 @@
         <v>5</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E5" si="0">"INSERT INTO p_g_programs VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"', "&amp;C4&amp;", "&amp;D4&amp;"');"</f>
-        <v>INSERT INTO p_g_programs VALUES('DIS','Master of Information Technology', null, null');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO p_g_programs VALUES('MITEC','Master of Information Technology',' null',' null');</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -5001,65 +5099,47 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO p_g_programs VALUES('DLIS','Master of Library and Information Science', null, null');</v>
+        <v>INSERT INTO p_g_programs VALUES('MLIB','Master of Library and Information Science',' null',' null');</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="str">
-        <f>"INSERT INTO p_g_programs VALUES('"&amp;A6&amp;"','"&amp;B6&amp;"', "&amp;C6&amp;", "&amp;D6&amp;"');"</f>
-        <v>INSERT INTO p_g_programs VALUES('DLIS','Doctor of Philosophy (Library and Information Science)', null, null');</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="15"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="15"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="15"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="15"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update date date for sem 2 2023-2024
</commit_message>
<xml_diff>
--- a/database/KICT Backup DB/Insert_Query.xlsx
+++ b/database/KICT Backup DB/Insert_Query.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/kict/database/KICT Backup DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1298BB2E-6862-FA4D-A6AA-1E3CA0E9F190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2BBF7-090A-2243-9595-DEB795F1B4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="1" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12700" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="307">
   <si>
     <t>staff_id</t>
   </si>
@@ -162,9 +162,6 @@
     <t>NOOR HAYANI BINTI ABD RAHIM</t>
   </si>
   <si>
-    <t>NOOR SHAFINI MOHAMAD</t>
-  </si>
-  <si>
     <t>NURAZLIN BINTI ZAINAL AZMI</t>
   </si>
   <si>
@@ -952,6 +949,18 @@
   </si>
   <si>
     <t>BUSINESS CONTINUITY AND DISASTER RECOVERY</t>
+  </si>
+  <si>
+    <t>INFO 4332</t>
+  </si>
+  <si>
+    <t>KNOWLEDGE MANAGEMENT PRACTICES AND APPLICATION</t>
+  </si>
+  <si>
+    <t>INFO 4313</t>
+  </si>
+  <si>
+    <t>DATA MINING</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1039,10 +1048,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1373,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050F0502-707F-E94C-BAD9-F21BCE0BBD9A}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1388,10 +1393,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1436,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">"INSERT INTO staff VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;");"</f>
+        <f t="shared" ref="E3:E65" si="0">"INSERT INTO staff VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;");"</f>
         <v>INSERT INTO staff VALUES('1716','ABD. RAHMAN BIN AHLAN', null, null);</v>
       </c>
     </row>
@@ -1945,10 +1950,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>6288</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="4">
+        <v>10163</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1959,12 +1964,12 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('6288','NOOR SHAFINI MOHAMAD', null, null);</v>
+        <v>INSERT INTO staff VALUES('10163','NURAZLIN BINTI ZAINAL AZMI', null, null);</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>10163</v>
+        <v>9026</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>41</v>
@@ -1977,12 +1982,12 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('10163','NURAZLIN BINTI ZAINAL AZMI', null, null);</v>
+        <v>INSERT INTO staff VALUES('9026','NURHAFIZAH BINTI MAHRI', null, null);</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>9026</v>
+        <v>5341</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>42</v>
@@ -1995,12 +2000,12 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('9026','NURHAFIZAH BINTI MAHRI', null, null);</v>
+        <v>INSERT INTO staff VALUES('5341','NURUL NUHA BINTI ABDUL MOLOK', null, null);</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>5341</v>
+        <v>4295</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>43</v>
@@ -2013,12 +2018,12 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('5341','NURUL NUHA BINTI ABDUL MOLOK', null, null);</v>
+        <v>INSERT INTO staff VALUES('4295','SHUHAILI BT. TALIB', null, null);</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>4295</v>
+        <v>6993</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>44</v>
@@ -2031,12 +2036,12 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4295','SHUHAILI BT. TALIB', null, null);</v>
+        <v>INSERT INTO staff VALUES('6993','SUHAILA BINTI SAMSURI', null, null);</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>6993</v>
+        <v>6948</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>45</v>
@@ -2049,12 +2054,12 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('6993','SUHAILA BINTI SAMSURI', null, null);</v>
+        <v>INSERT INTO staff VALUES('6948','ZAHIDAH BINTI ZULKIFLI', null, null);</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>6948</v>
+        <v>4896</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>46</v>
@@ -2067,15 +2072,15 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('6948','ZAHIDAH BINTI ZULKIFLI', null, null);</v>
+        <v>INSERT INTO staff VALUES('4896','ZAINATUL SHIMA ABDULLAH', null, null);</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
-        <v>4896</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>47</v>
+      <c r="A39" s="9">
+        <v>7132</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -2085,14 +2090,14 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4896','ZAINATUL SHIMA ABDULLAH', null, null);</v>
+        <v>INSERT INTO staff VALUES('7132','ADAMU ABUBAKAR IBRAHIM', null, null);</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
-        <v>7132</v>
-      </c>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="9">
+        <v>10332</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>112</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2103,14 +2108,14 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('7132','ADAMU ABUBAKAR IBRAHIM', null, null);</v>
+        <v>INSERT INTO staff VALUES('10332','AHSIAH BINTI ISMAIL', null, null);</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="11">
-        <v>10332</v>
-      </c>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="9">
+        <v>9608</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2121,14 +2126,14 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('10332','AHSIAH BINTI ISMAIL', null, null);</v>
+        <v>INSERT INTO staff VALUES('9608','AKEEM OLOWOLAYEMO', null, null);</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
-        <v>9608</v>
-      </c>
-      <c r="B42" s="12" t="s">
+      <c r="A42" s="9">
+        <v>4296</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>114</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2139,14 +2144,14 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('9608','AKEEM OLOWOLAYEMO', null, null);</v>
+        <v>INSERT INTO staff VALUES('4296','AMELIA RITAHANI BT. ISMAIL', null, null);</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="11">
-        <v>4296</v>
-      </c>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="9">
+        <v>9221</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>115</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2157,14 +2162,14 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4296','AMELIA RITAHANI BT. ISMAIL', null, null);</v>
+        <v>INSERT INTO staff VALUES('9221','AMIR AATIEFF BIN AMIR HUSSIN', null, null);</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="11">
-        <v>9221</v>
-      </c>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="9">
+        <v>9157</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>116</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2175,14 +2180,14 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('9221','AMIR AATIEFF BIN AMIR HUSSIN', null, null);</v>
+        <v>INSERT INTO staff VALUES('9157','ANDI FITRIAH BINTI ABDUL KADIR', null, null);</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="11">
-        <v>9157</v>
-      </c>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="9">
+        <v>10324</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>117</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2193,14 +2198,14 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('9157','ANDI FITRIAH BINTI ABDUL KADIR', null, null);</v>
+        <v>INSERT INTO staff VALUES('10324','ASMARANI BINTI AHMAD PUZI', null, null);</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="11">
-        <v>10324</v>
-      </c>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="9">
+        <v>5133</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>118</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2211,14 +2216,14 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('10324','ASMARANI BINTI AHMAD PUZI', null, null);</v>
+        <v>INSERT INTO staff VALUES('5133','AZLIN BINTI NORDIN', null, null);</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="11">
-        <v>5133</v>
-      </c>
-      <c r="B47" s="12" t="s">
+      <c r="A47" s="9">
+        <v>10567</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>119</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2229,14 +2234,14 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('5133','AZLIN BINTI NORDIN', null, null);</v>
+        <v>INSERT INTO staff VALUES('10567','DINI OKTARINA DWI HANDAYANI', null, null);</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="11">
-        <v>10567</v>
-      </c>
-      <c r="B48" s="12" t="s">
+      <c r="A48" s="9">
+        <v>7910</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>120</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -2247,14 +2252,14 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('10567','DINI OKTARINA DWI HANDAYANI', null, null);</v>
+        <v>INSERT INTO staff VALUES('7910','HAFIZAH BINTI MANSOR', null, null);</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="11">
-        <v>7910</v>
-      </c>
-      <c r="B49" s="12" t="s">
+      <c r="A49" s="9">
+        <v>4870</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>121</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2265,14 +2270,14 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('7910','HAFIZAH BINTI MANSOR', null, null);</v>
+        <v>INSERT INTO staff VALUES('4870','HAMWIRA SAKTI BIN YAACOB', null, null);</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="11">
-        <v>4870</v>
-      </c>
-      <c r="B50" s="12" t="s">
+      <c r="A50" s="9">
+        <v>771</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2283,14 +2288,14 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4870','HAMWIRA SAKTI BIN YAACOB', null, null);</v>
+        <v>INSERT INTO staff VALUES('771','MAZNAH BT AHMAD', null, null);</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="11">
-        <v>771</v>
-      </c>
-      <c r="B51" s="12" t="s">
+      <c r="A51" s="9">
+        <v>8123</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2301,14 +2306,14 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('771','MAZNAH BT AHMAD', null, null);</v>
+        <v>INSERT INTO staff VALUES('8123','NORBIK BASHAH BIN IDRIS', null, null);</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="11">
-        <v>8123</v>
-      </c>
-      <c r="B52" s="12" t="s">
+      <c r="A52" s="9">
+        <v>9622</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2319,14 +2324,14 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8123','NORBIK BASHAH BIN IDRIS', null, null);</v>
+        <v>INSERT INTO staff VALUES('9622','NORLIA MD YUSOF', null, null);</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="11">
-        <v>9622</v>
-      </c>
-      <c r="B53" s="12" t="s">
+      <c r="A53" s="9">
+        <v>5505</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2337,14 +2342,14 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('9622','NORLIA MD YUSOF', null, null);</v>
+        <v>INSERT INTO staff VALUES('5505','NORMAZIAH BINTI ABDUL AZIZ', null, null);</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="11">
-        <v>5505</v>
-      </c>
-      <c r="B54" s="12" t="s">
+      <c r="A54" s="9">
+        <v>3509</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>126</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2355,14 +2360,14 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('5505','NORMAZIAH BINTI ABDUL AZIZ', null, null);</v>
+        <v>INSERT INTO staff VALUES('3509','NORMI SHAM BT. AWANG ABU BAKAR', null, null);</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="11">
-        <v>3509</v>
-      </c>
-      <c r="B55" s="12" t="s">
+      <c r="A55" s="9">
+        <v>3705</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>127</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2373,14 +2378,14 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('3509','NORMI SHAM BT. AWANG ABU BAKAR', null, null);</v>
+        <v>INSERT INTO staff VALUES('3705','NORSAREMAH BT. SALLEH', null, null);</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="11">
-        <v>3705</v>
-      </c>
-      <c r="B56" s="12" t="s">
+      <c r="A56" s="9">
+        <v>8627</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>128</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -2391,14 +2396,14 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('3705','NORSAREMAH BT. SALLEH', null, null);</v>
+        <v>INSERT INTO staff VALUES('8627','NORZALIZA BINTI MD NOR', null, null);</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="11">
-        <v>8627</v>
-      </c>
-      <c r="B57" s="12" t="s">
+      <c r="A57" s="9">
+        <v>8405</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2409,14 +2414,14 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8627','NORZALIZA BINTI MD NOR', null, null);</v>
+        <v>INSERT INTO staff VALUES('8405','NOOR AZURA BINTI ZAKARIA', null, null);</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="11">
-        <v>8405</v>
-      </c>
-      <c r="B58" s="12" t="s">
+      <c r="A58" s="9">
+        <v>5066</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>130</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2427,14 +2432,14 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8405','NOOR AZURA BINTI ZAKARIA', null, null);</v>
+        <v>INSERT INTO staff VALUES('5066','NORZARIYAH BINTI YAHYA', null, null);</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="11">
-        <v>5066</v>
-      </c>
-      <c r="B59" s="12" t="s">
+      <c r="A59" s="9">
+        <v>8371</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>131</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2445,14 +2450,14 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('5066','NORZARIYAH BINTI YAHYA', null, null);</v>
+        <v>INSERT INTO staff VALUES('8371','NURUL LIYANA BINTI MOHAMAD ZULKUFLI', null, null);</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="11">
-        <v>8371</v>
-      </c>
-      <c r="B60" s="12" t="s">
+      <c r="A60" s="9">
+        <v>4964</v>
+      </c>
+      <c r="B60" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2463,14 +2468,14 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8371','NURUL LIYANA BINTI MOHAMAD ZULKUFLI', null, null);</v>
+        <v>INSERT INTO staff VALUES('4964','RAINI BINTI HASSAN', null, null);</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="11">
-        <v>4964</v>
-      </c>
-      <c r="B61" s="12" t="s">
+      <c r="A61" s="9">
+        <v>8638</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -2481,14 +2486,14 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4964','RAINI BINTI HASSAN', null, null);</v>
+        <v>INSERT INTO staff VALUES('8638','RAWAD ABDULKHALEQ ABDULMOLLA ABDULGHAFOR', null, null);</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="11">
-        <v>8638</v>
-      </c>
-      <c r="B62" s="12" t="s">
+      <c r="A62" s="9">
+        <v>5251</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>134</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2499,14 +2504,14 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8638','RAWAD ABDULKHALEQ ABDULMOLLA ABDULGHAFOR', null, null);</v>
+        <v>INSERT INTO staff VALUES('5251','RIZAL BIN MOHD. NOR', null, null);</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="11">
-        <v>5251</v>
-      </c>
-      <c r="B63" s="12" t="s">
+      <c r="A63" s="9">
+        <v>8667</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>135</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -2517,14 +2522,14 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('5251','RIZAL BIN MOHD. NOR', null, null);</v>
+        <v>INSERT INTO staff VALUES('8667','SHARYAR WANI', null, null);</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="11">
-        <v>8667</v>
-      </c>
-      <c r="B64" s="12" t="s">
+      <c r="A64" s="9">
+        <v>7620</v>
+      </c>
+      <c r="B64" s="10" t="s">
         <v>136</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -2535,14 +2540,14 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('8667','SHARYAR WANI', null, null);</v>
+        <v>INSERT INTO staff VALUES('7620','SITI ASMA BINTI MOHAMMED', null, null);</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="11">
-        <v>7620</v>
-      </c>
-      <c r="B65" s="12" t="s">
+      <c r="A65" s="9">
+        <v>4615</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>137</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -2553,14 +2558,14 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('7620','SITI ASMA BINTI MOHAMMED', null, null);</v>
+        <v>INSERT INTO staff VALUES('4615','SURIANI BT. SULAIMAN', null, null);</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="11">
-        <v>4615</v>
-      </c>
-      <c r="B66" s="12" t="s">
+      <c r="A66" s="9">
+        <v>9954</v>
+      </c>
+      <c r="B66" s="10" t="s">
         <v>138</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2570,15 +2575,15 @@
         <v>5</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO staff VALUES('4615','SURIANI BT. SULAIMAN', null, null);</v>
+        <f t="shared" ref="E66:E76" si="1">"INSERT INTO staff VALUES('"&amp;A66&amp;"','"&amp;B66&amp;"', "&amp;C66&amp;", "&amp;D66&amp;");"</f>
+        <v>INSERT INTO staff VALUES('9954','TAKUMI SASE', null, null);</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="11">
-        <v>9954</v>
-      </c>
-      <c r="B67" s="12" t="s">
+      <c r="A67" s="9">
+        <v>10552</v>
+      </c>
+      <c r="B67" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2588,15 +2593,15 @@
         <v>5</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E77" si="1">"INSERT INTO staff VALUES('"&amp;A67&amp;"','"&amp;B67&amp;"', "&amp;C67&amp;", "&amp;D67&amp;");"</f>
-        <v>INSERT INTO staff VALUES('9954','TAKUMI SASE', null, null);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO staff VALUES('10552','ZAINAB SENAN MAHMOD ATTAR BASHI', null, null);</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="11">
-        <v>10552</v>
-      </c>
-      <c r="B68" s="12" t="s">
+      <c r="A68" s="9">
+        <v>10744</v>
+      </c>
+      <c r="B68" s="10" t="s">
         <v>140</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2607,14 +2612,14 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('10552','ZAINAB SENAN MAHMOD ATTAR BASHI', null, null);</v>
+        <v>INSERT INTO staff VALUES('10744','TENGKU MOHD BIN TENGKU SEMBOK ', null, null);</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="11">
-        <v>10744</v>
-      </c>
-      <c r="B69" s="12" t="s">
+      <c r="A69" s="9">
+        <v>10738</v>
+      </c>
+      <c r="B69" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -2625,14 +2630,14 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('10744','TENGKU MOHD BIN TENGKU SEMBOK ', null, null);</v>
+        <v>INSERT INTO staff VALUES('10738','AHMAD ANWAR BIN ZAINUDDIN', null, null);</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="11">
-        <v>10738</v>
-      </c>
-      <c r="B70" s="12" t="s">
+      <c r="A70" s="9">
+        <v>10722</v>
+      </c>
+      <c r="B70" s="10" t="s">
         <v>142</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2643,15 +2648,15 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('10738','AHMAD ANWAR BIN ZAINUDDIN', null, null);</v>
+        <v>INSERT INTO staff VALUES('10722','ABDUL WAHAB BIN ABDUL RAHMAN', null, null);</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="11">
-        <v>10722</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>143</v>
+      <c r="A71" s="2">
+        <v>1675</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>293</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>5</v>
@@ -2661,14 +2666,14 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('10722','ABDUL WAHAB BIN ABDUL RAHMAN', null, null);</v>
+        <v>INSERT INTO staff VALUES('1675','ROSLINA OTHMAN ', null, null);</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>1675</v>
-      </c>
-      <c r="B72" s="12" t="s">
+        <v>7684</v>
+      </c>
+      <c r="B72" s="10" t="s">
         <v>294</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -2679,14 +2684,14 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('1675','ROSLINA OTHMAN ', null, null);</v>
+        <v>INSERT INTO staff VALUES('7684','ROOSFA HASHIM', null, null);</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>7684</v>
-      </c>
-      <c r="B73" s="12" t="s">
+        <v>8227</v>
+      </c>
+      <c r="B73" s="10" t="s">
         <v>295</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -2697,14 +2702,14 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('7684','ROOSFA HASHIM', null, null);</v>
+        <v>INSERT INTO staff VALUES('8227','SHARIFAH NUR AMIRAH SARIF ABDULLAH', null, null);</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>8227</v>
-      </c>
-      <c r="B74" s="12" t="s">
+        <v>9019</v>
+      </c>
+      <c r="B74" s="10" t="s">
         <v>296</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -2715,14 +2720,14 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('8227','SHARIFAH NUR AMIRAH SARIF ABDULLAH', null, null);</v>
+        <v>INSERT INTO staff VALUES('9019','NOR SAADAH MD. NOR', null, null);</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>9019</v>
-      </c>
-      <c r="B75" s="12" t="s">
+        <v>9041</v>
+      </c>
+      <c r="B75" s="10" t="s">
         <v>297</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -2733,14 +2738,14 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('9019','NOR SAADAH MD. NOR', null, null);</v>
+        <v>INSERT INTO staff VALUES('9041','NUR LEYNI NILAM PUTRI JUNURHAM', null, null);</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>9041</v>
-      </c>
-      <c r="B76" s="12" t="s">
+        <v>11085</v>
+      </c>
+      <c r="B76" s="10" t="s">
         <v>298</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -2750,24 +2755,6 @@
         <v>5</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO staff VALUES('9041','NUR LEYNI NILAM PUTRI JUNURHAM', null, null);</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
-        <v>11085</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO staff VALUES('11085','AYUB BIN ABDUL RAHMAN', null, null);</v>
       </c>
@@ -2780,10 +2767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63454FF6-7634-A745-9553-1678A6EECCD5}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2815,11 +2802,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -2836,11 +2823,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -2852,16 +2839,16 @@
         <v>9</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F67" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;", '"&amp;E3&amp;"');"</f>
+        <f t="shared" ref="F3:F69" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;", '"&amp;E3&amp;"');"</f>
         <v>INSERT INTO courses VALUES('INFO 1302','BUSINESS FUNDAMENTALS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -2878,11 +2865,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -2899,11 +2886,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -2920,11 +2907,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -2941,11 +2928,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -2962,11 +2949,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -2983,11 +2970,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -3004,11 +2991,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -3025,11 +3012,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -3046,11 +3033,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -3067,11 +3054,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -3088,11 +3075,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -3109,11 +3096,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -3130,11 +3117,11 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -3151,11 +3138,11 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -3172,11 +3159,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>83</v>
+      <c r="A19" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -3189,15 +3176,15 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4314','BUSINESS DATA ANALYTICS', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4313','DATA MINING', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>85</v>
+      <c r="A20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -3210,15 +3197,15 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4320','ANIMATION TECHNIQUE', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4314','BUSINESS DATA ANALYTICS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>87</v>
+      <c r="A21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -3231,15 +3218,15 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4321','CREATIVE DESIGN TECHNIQUES', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4320','ANIMATION TECHNIQUE', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>89</v>
+      <c r="A22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -3252,15 +3239,15 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4325','GRAPHIC DESIGN', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4321','CREATIVE DESIGN TECHNIQUES', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>91</v>
+      <c r="A23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -3273,15 +3260,15 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4328','GAME DESIGN AND DEVELOPMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4325','GRAPHIC DESIGN', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>93</v>
+      <c r="A24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -3294,15 +3281,15 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4333','INTEGRATED BUSINESS PROCESS AND ERP SYSTEMS', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4328','GAME DESIGN AND DEVELOPMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>95</v>
+      <c r="A25" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>304</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -3315,15 +3302,15 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4335','MOBILE APPLICATION DEVELOPMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4332','KNOWLEDGE MANAGEMENT PRACTICES AND APPLICATION', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>97</v>
+      <c r="A26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -3336,15 +3323,15 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4336','INFORMATION RETRIEVAL TECHNOLOGIES', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4333','INTEGRATED BUSINESS PROCESS AND ERP SYSTEMS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>99</v>
+      <c r="A27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -3357,15 +3344,15 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4330','CONTROL AND AUDIT OF INFORMATION SYSTEMS', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4335','MOBILE APPLICATION DEVELOPMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>101</v>
+      <c r="A28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -3378,15 +3365,15 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4340','MANAGEMENT OF INFORMATION SECURITY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4336','INFORMATION RETRIEVAL TECHNOLOGIES', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>103</v>
+      <c r="A29" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -3399,15 +3386,15 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4341','RISK MANAGEMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4330','CONTROL AND AUDIT OF INFORMATION SYSTEMS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>303</v>
+      <c r="A30" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -3420,15 +3407,15 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4342','BUSINESS CONTINUITY AND DISASTER RECOVERY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4340','MANAGEMENT OF INFORMATION SECURITY', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>105</v>
+      <c r="A31" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -3441,15 +3428,15 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4343','INFORMATION PRIVACY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4341','RISK MANAGEMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>107</v>
+      <c r="A32" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -3462,15 +3449,15 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4351','DIGITALPRENEURSHIP', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4342','BUSINESS CONTINUITY AND DISASTER RECOVERY', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>109</v>
+      <c r="A33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -3483,761 +3470,803 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('INFO 4343','INFORMATION PRIVACY', null, null, 'BIT');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('INFO 4351','DIGITALPRENEURSHIP', null, null, 'BIT');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO courses VALUES('INFO 4352','DIGITALPRENEURSHIP CUSTOMER DEVELOPMENT', null, null, 'BIT');</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1300','ELEMENTS OF PROGRAMMING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1301','OBJECT ORIENTED PROGRAMMING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1302','INTRODUCTION TO COMPUTER ORGANIZATION', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1303','MATHEMATICS FOR COMPUTING I', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1304','PROBABILITY AND STATISTICS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 1305','INTRODUCTION TO SOFTWARE ENGINEERING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1300','ELEMENTS OF PROGRAMMING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1301','OBJECT ORIENTED PROGRAMMING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1302','INTRODUCTION TO COMPUTER ORGANIZATION', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B37" s="12" t="s">
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2300','DATA STRUCTURES AND ALGORITHMS I', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2301','COMPUTER NETWORKING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2302','DIGITAL SYSTEMS FUNDAMENTALS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2303','PRINCIPLE OF IT SECURITY', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2304','INTELLIGENT SYSTEMS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 2305','MATHEMATICS FOR COMPUTING II', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 3300','OPERATING SYSTEMS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 3301','COMPUTER ARCHITECTURE AND ASSEMBLY LANGUAGE', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 3302','DATA STRUCTURES AND ALGORITHMS II', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 3303','MATHEMATICS FOR COMPUTING III', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4300','COMPUTATION AND COMPLEXITY', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4312','BLOCKCHAIN &amp; APPLICATION', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4320','SOFTWARE TESTING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4321','PROJECT MANAGEMENT IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4322','SOFTWARE DESIGN AND ARCHITECTURE', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4323','REQUIREMENTS ENGINEERING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4330','NETWORKING CONCEPTS AND PRACTICES', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4331','ENTERPRISE NETWORK', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4332','DIGITAL EVIDENCE FORENSICS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4333','CRYPTOGRAPHY', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4336','NETWORK SECURITY', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4340','MACHINE LEARNING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4341','BIG DATA ANALYTICS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4342','NATURAL LANGUAGE PROCESSING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4343','DATA SCIENCE', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4346','BIOINSPIRED COMPUTING', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4347','BRAIN COMPUTATIONAL ANALYTICS', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4311','MOBILE APPLICATION DEVELOPMENT', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" ref="F70:F71" si="1">"INSERT INTO courses VALUES('"&amp;A70&amp;"','"&amp;B70&amp;"', "&amp;C70&amp;", "&amp;D70&amp;", '"&amp;E70&amp;"');"</f>
+        <v>INSERT INTO courses VALUES('CSCI 4325','SOFTWARE QUALITY ASSURANCE', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1303','MATHEMATICS FOR COMPUTING I', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1304','PROBABILITY AND STATISTICS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
+      <c r="C71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1305','INTRODUCTION TO SOFTWARE ENGINEERING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2300','DATA STRUCTURES AND ALGORITHMS I', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2301','COMPUTER NETWORKING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2302','DIGITAL SYSTEMS FUNDAMENTALS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2303','PRINCIPLE OF IT SECURITY', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2304','INTELLIGENT SYSTEMS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2305','MATHEMATICS FOR COMPUTING II', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3300','OPERATING SYSTEMS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3301','COMPUTER ARCHITECTURE AND ASSEMBLY LANGUAGE', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F48" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3302','DATA STRUCTURES AND ALGORITHMS II', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3303','MATHEMATICS FOR COMPUTING III', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4300','COMPUTATION AND COMPLEXITY', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F51" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4312','BLOCKCHAIN &amp; APPLICATION', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4320','SOFTWARE TESTING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4321','PROJECT MANAGEMENT IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4322','SOFTWARE DESIGN AND ARCHITECTURE', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F55" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4323','REQUIREMENTS ENGINEERING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F56" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4330','NETWORKING CONCEPTS AND PRACTICES', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F57" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4331','ENTERPRISE NETWORK', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F58" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4332','DIGITAL EVIDENCE FORENSICS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4333','CRYPTOGRAPHY', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4336','NETWORK SECURITY', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4340','MACHINE LEARNING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4341','BIG DATA ANALYTICS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4342','NATURAL LANGUAGE PROCESSING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4343','DATA SCIENCE', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4346','BIOINSPIRED COMPUTING', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4347','BRAIN COMPUTATIONAL ANALYTICS', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F67" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4311','MOBILE APPLICATION DEVELOPMENT', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F68" t="str">
-        <f t="shared" ref="F68:F69" si="1">"INSERT INTO courses VALUES('"&amp;A68&amp;"','"&amp;B68&amp;"', "&amp;C68&amp;", "&amp;D68&amp;", '"&amp;E68&amp;"');"</f>
-        <v>INSERT INTO courses VALUES('CSCI 4325','SOFTWARE QUALITY ASSURANCE', null, null, 'BCS');</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F69" t="str">
+      <c r="F71" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO courses VALUES('CSCI 4326','EMPIRICAL METHODS IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
       </c>
@@ -4285,11 +4314,11 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
         <v>219</v>
       </c>
-      <c r="B2" t="s">
-        <v>220</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4297,7 +4326,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F2" t="str">
         <f>"INSERT INTO courses VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"', "&amp;C2&amp;", "&amp;D2&amp;", '"&amp;E2&amp;"');"</f>
@@ -4306,11 +4335,11 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" t="s">
         <v>221</v>
       </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
@@ -4318,7 +4347,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F37" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;", '"&amp;E3&amp;"');"</f>
@@ -4327,11 +4356,11 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
         <v>223</v>
       </c>
-      <c r="B4" t="s">
-        <v>224</v>
-      </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
@@ -4339,7 +4368,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -4348,11 +4377,11 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
         <v>225</v>
       </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
@@ -4360,7 +4389,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -4369,11 +4398,11 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" t="s">
         <v>227</v>
       </c>
-      <c r="B6" t="s">
-        <v>228</v>
-      </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -4381,7 +4410,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -4390,11 +4419,11 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" t="s">
         <v>229</v>
       </c>
-      <c r="B7" t="s">
-        <v>230</v>
-      </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
@@ -4402,7 +4431,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -4411,11 +4440,11 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" t="s">
         <v>231</v>
       </c>
-      <c r="B8" t="s">
-        <v>232</v>
-      </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -4423,7 +4452,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -4432,11 +4461,11 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" t="s">
         <v>233</v>
       </c>
-      <c r="B9" t="s">
-        <v>234</v>
-      </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
@@ -4444,7 +4473,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -4453,11 +4482,11 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
         <v>235</v>
       </c>
-      <c r="B10" t="s">
-        <v>236</v>
-      </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
@@ -4465,7 +4494,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -4474,11 +4503,11 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" t="s">
         <v>237</v>
       </c>
-      <c r="B11" t="s">
-        <v>238</v>
-      </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
@@ -4486,7 +4515,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -4495,11 +4524,11 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" t="s">
         <v>239</v>
       </c>
-      <c r="B12" t="s">
-        <v>240</v>
-      </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
@@ -4507,7 +4536,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -4516,11 +4545,11 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" t="s">
         <v>241</v>
       </c>
-      <c r="B13" t="s">
-        <v>242</v>
-      </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
@@ -4528,7 +4557,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -4537,11 +4566,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" t="s">
         <v>243</v>
       </c>
-      <c r="B14" t="s">
-        <v>244</v>
-      </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
@@ -4549,7 +4578,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -4558,11 +4587,11 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" t="s">
         <v>245</v>
       </c>
-      <c r="B15" t="s">
-        <v>246</v>
-      </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
@@ -4570,7 +4599,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -4579,11 +4608,11 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
         <v>247</v>
       </c>
-      <c r="B16" t="s">
-        <v>248</v>
-      </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
@@ -4591,7 +4620,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -4600,10 +4629,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -4612,7 +4641,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -4621,11 +4650,11 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B18" t="s">
         <v>250</v>
       </c>
-      <c r="B18" t="s">
-        <v>251</v>
-      </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
@@ -4633,7 +4662,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -4642,10 +4671,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -4654,7 +4683,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -4663,10 +4692,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -4675,7 +4704,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -4684,10 +4713,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -4696,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -4705,10 +4734,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -4717,7 +4746,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -4726,10 +4755,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -4738,7 +4767,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -4747,10 +4776,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -4759,7 +4788,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -4768,10 +4797,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -4780,7 +4809,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -4789,10 +4818,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -4801,7 +4830,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -4810,11 +4839,11 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B27" t="s">
         <v>268</v>
       </c>
-      <c r="B27" t="s">
-        <v>269</v>
-      </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
       </c>
@@ -4822,7 +4851,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -4831,10 +4860,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -4843,7 +4872,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -4852,10 +4881,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -4864,7 +4893,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -4873,10 +4902,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -4885,7 +4914,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -4894,10 +4923,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -4906,7 +4935,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -4915,11 +4944,11 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" t="s">
         <v>272</v>
       </c>
-      <c r="B32" t="s">
-        <v>273</v>
-      </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +4956,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -4936,10 +4965,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -4948,7 +4977,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -4957,10 +4986,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -4969,7 +4998,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -4978,11 +5007,11 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B35" t="s">
         <v>275</v>
       </c>
-      <c r="B35" t="s">
-        <v>276</v>
-      </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
       </c>
@@ -4990,7 +5019,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -4999,11 +5028,11 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B36" t="s">
         <v>277</v>
       </c>
-      <c r="B36" t="s">
-        <v>278</v>
-      </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
@@ -5011,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -5020,11 +5049,11 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B37" t="s">
         <v>279</v>
       </c>
-      <c r="B37" t="s">
-        <v>280</v>
-      </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5061,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -5066,7 +5095,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -5079,11 +5108,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>289</v>
+      <c r="A2" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -5097,11 +5126,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>300</v>
+      <c r="A3" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>299</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -5116,10 +5145,10 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>288</v>
+        <v>291</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -5134,10 +5163,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -5207,22 +5236,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update course 3d modelling
</commit_message>
<xml_diff>
--- a/database/KICT Backup DB/Insert_Query.xlsx
+++ b/database/KICT Backup DB/Insert_Query.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/kict/database/KICT Backup DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2BBF7-090A-2243-9595-DEB795F1B4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA52919-64A6-D44C-B96F-622BEDBFC151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12700" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12700" activeTab="1" xr2:uid="{D96C4D52-B7C3-BB4A-B012-D6CB397DAC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="309">
   <si>
     <t>staff_id</t>
   </si>
@@ -961,6 +961,12 @@
   </si>
   <si>
     <t>DATA MINING</t>
+  </si>
+  <si>
+    <t>INFO 4326</t>
+  </si>
+  <si>
+    <t>3D MODELLING</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050F0502-707F-E94C-BAD9-F21BCE0BBD9A}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="125" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -2767,10 +2773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63454FF6-7634-A745-9553-1678A6EECCD5}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2839,7 +2845,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F69" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;", '"&amp;E3&amp;"');"</f>
+        <f t="shared" ref="F3:F70" si="0">"INSERT INTO courses VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"', "&amp;C3&amp;", "&amp;D3&amp;", '"&amp;E3&amp;"');"</f>
         <v>INSERT INTO courses VALUES('INFO 1302','BUSINESS FUNDAMENTALS', null, null, 'BIT');</v>
       </c>
     </row>
@@ -3265,10 +3271,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>89</v>
+        <v>307</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>90</v>
+        <v>308</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -3281,15 +3287,15 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4328','GAME DESIGN AND DEVELOPMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4326','3D MODELLING', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>303</v>
+        <v>89</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>304</v>
+        <v>90</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -3302,15 +3308,15 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4332','KNOWLEDGE MANAGEMENT PRACTICES AND APPLICATION', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4328','GAME DESIGN AND DEVELOPMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>91</v>
+        <v>303</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>92</v>
+        <v>304</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -3323,15 +3329,15 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4333','INTEGRATED BUSINESS PROCESS AND ERP SYSTEMS', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4332','KNOWLEDGE MANAGEMENT PRACTICES AND APPLICATION', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -3344,15 +3350,15 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4335','MOBILE APPLICATION DEVELOPMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4333','INTEGRATED BUSINESS PROCESS AND ERP SYSTEMS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -3365,15 +3371,15 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4336','INFORMATION RETRIEVAL TECHNOLOGIES', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4335','MOBILE APPLICATION DEVELOPMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -3386,15 +3392,15 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4330','CONTROL AND AUDIT OF INFORMATION SYSTEMS', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4336','INFORMATION RETRIEVAL TECHNOLOGIES', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -3407,15 +3413,15 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4340','MANAGEMENT OF INFORMATION SECURITY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4330','CONTROL AND AUDIT OF INFORMATION SYSTEMS', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -3428,15 +3434,15 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4341','RISK MANAGEMENT', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4340','MANAGEMENT OF INFORMATION SECURITY', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>301</v>
+        <v>101</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>302</v>
+        <v>102</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -3449,15 +3455,15 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4342','BUSINESS CONTINUITY AND DISASTER RECOVERY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4341','RISK MANAGEMENT', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>103</v>
+        <v>301</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>104</v>
+        <v>302</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -3470,15 +3476,15 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4343','INFORMATION PRIVACY', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4342','BUSINESS CONTINUITY AND DISASTER RECOVERY', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -3491,15 +3497,15 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('INFO 4351','DIGITALPRENEURSHIP', null, null, 'BIT');</v>
+        <v>INSERT INTO courses VALUES('INFO 4343','INFORMATION PRIVACY', null, null, 'BIT');</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -3512,36 +3518,36 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('INFO 4351','DIGITALPRENEURSHIP', null, null, 'BIT');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO courses VALUES('INFO 4352','DIGITALPRENEURSHIP CUSTOMER DEVELOPMENT', null, null, 'BIT');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1300','ELEMENTS OF PROGRAMMING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -3554,15 +3560,15 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1301','OBJECT ORIENTED PROGRAMMING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1300','ELEMENTS OF PROGRAMMING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -3575,15 +3581,15 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1302','INTRODUCTION TO COMPUTER ORGANIZATION', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1301','OBJECT ORIENTED PROGRAMMING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -3596,15 +3602,15 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1303','MATHEMATICS FOR COMPUTING I', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1302','INTRODUCTION TO COMPUTER ORGANIZATION', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>5</v>
@@ -3617,15 +3623,15 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1304','PROBABILITY AND STATISTICS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1303','MATHEMATICS FOR COMPUTING I', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>5</v>
@@ -3638,15 +3644,15 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 1305','INTRODUCTION TO SOFTWARE ENGINEERING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1304','PROBABILITY AND STATISTICS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>5</v>
@@ -3659,15 +3665,15 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2300','DATA STRUCTURES AND ALGORITHMS I', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 1305','INTRODUCTION TO SOFTWARE ENGINEERING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>5</v>
@@ -3680,15 +3686,15 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2301','COMPUTER NETWORKING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2300','DATA STRUCTURES AND ALGORITHMS I', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>5</v>
@@ -3701,15 +3707,15 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2302','DIGITAL SYSTEMS FUNDAMENTALS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2301','COMPUTER NETWORKING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>5</v>
@@ -3722,15 +3728,15 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2303','PRINCIPLE OF IT SECURITY', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2302','DIGITAL SYSTEMS FUNDAMENTALS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>5</v>
@@ -3743,15 +3749,15 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2304','INTELLIGENT SYSTEMS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2303','PRINCIPLE OF IT SECURITY', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>5</v>
@@ -3764,15 +3770,15 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 2305','MATHEMATICS FOR COMPUTING II', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2304','INTELLIGENT SYSTEMS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>5</v>
@@ -3785,15 +3791,15 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3300','OPERATING SYSTEMS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 2305','MATHEMATICS FOR COMPUTING II', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>5</v>
@@ -3806,15 +3812,15 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3301','COMPUTER ARCHITECTURE AND ASSEMBLY LANGUAGE', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 3300','OPERATING SYSTEMS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>5</v>
@@ -3827,15 +3833,15 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3302','DATA STRUCTURES AND ALGORITHMS II', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 3301','COMPUTER ARCHITECTURE AND ASSEMBLY LANGUAGE', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>5</v>
@@ -3848,15 +3854,15 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 3303','MATHEMATICS FOR COMPUTING III', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 3302','DATA STRUCTURES AND ALGORITHMS II', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>5</v>
@@ -3869,15 +3875,15 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4300','COMPUTATION AND COMPLEXITY', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 3303','MATHEMATICS FOR COMPUTING III', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>5</v>
@@ -3890,15 +3896,15 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4312','BLOCKCHAIN &amp; APPLICATION', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4300','COMPUTATION AND COMPLEXITY', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>5</v>
@@ -3911,15 +3917,15 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4320','SOFTWARE TESTING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4312','BLOCKCHAIN &amp; APPLICATION', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>5</v>
@@ -3932,15 +3938,15 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4321','PROJECT MANAGEMENT IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4320','SOFTWARE TESTING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>5</v>
@@ -3953,15 +3959,15 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4322','SOFTWARE DESIGN AND ARCHITECTURE', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4321','PROJECT MANAGEMENT IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
@@ -3974,15 +3980,15 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4323','REQUIREMENTS ENGINEERING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4322','SOFTWARE DESIGN AND ARCHITECTURE', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>5</v>
@@ -3995,15 +4001,15 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4330','NETWORKING CONCEPTS AND PRACTICES', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4323','REQUIREMENTS ENGINEERING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>5</v>
@@ -4016,15 +4022,15 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4331','ENTERPRISE NETWORK', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4330','NETWORKING CONCEPTS AND PRACTICES', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>5</v>
@@ -4037,15 +4043,15 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4332','DIGITAL EVIDENCE FORENSICS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4331','ENTERPRISE NETWORK', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>5</v>
@@ -4058,15 +4064,15 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4333','CRYPTOGRAPHY', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4332','DIGITAL EVIDENCE FORENSICS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
@@ -4079,15 +4085,15 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4336','NETWORK SECURITY', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4333','CRYPTOGRAPHY', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>5</v>
@@ -4100,15 +4106,15 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4340','MACHINE LEARNING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4336','NETWORK SECURITY', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>5</v>
@@ -4121,15 +4127,15 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4341','BIG DATA ANALYTICS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4340','MACHINE LEARNING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
@@ -4142,15 +4148,15 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4342','NATURAL LANGUAGE PROCESSING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4341','BIG DATA ANALYTICS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>5</v>
@@ -4163,15 +4169,15 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4343','DATA SCIENCE', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4342','NATURAL LANGUAGE PROCESSING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>5</v>
@@ -4184,15 +4190,15 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4346','BIOINSPIRED COMPUTING', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4343','DATA SCIENCE', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>5</v>
@@ -4205,15 +4211,15 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4347','BRAIN COMPUTATIONAL ANALYTICS', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4346','BIOINSPIRED COMPUTING', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>5</v>
@@ -4226,15 +4232,15 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO courses VALUES('CSCI 4311','MOBILE APPLICATION DEVELOPMENT', null, null, 'BCS');</v>
+        <v>INSERT INTO courses VALUES('CSCI 4347','BRAIN COMPUTATIONAL ANALYTICS', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>5</v>
@@ -4246,16 +4252,16 @@
         <v>184</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" ref="F70:F71" si="1">"INSERT INTO courses VALUES('"&amp;A70&amp;"','"&amp;B70&amp;"', "&amp;C70&amp;", "&amp;D70&amp;", '"&amp;E70&amp;"');"</f>
-        <v>INSERT INTO courses VALUES('CSCI 4325','SOFTWARE QUALITY ASSURANCE', null, null, 'BCS');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO courses VALUES('CSCI 4311','MOBILE APPLICATION DEVELOPMENT', null, null, 'BCS');</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>5</v>
@@ -4267,6 +4273,27 @@
         <v>184</v>
       </c>
       <c r="F71" t="str">
+        <f t="shared" ref="F71:F72" si="1">"INSERT INTO courses VALUES('"&amp;A71&amp;"','"&amp;B71&amp;"', "&amp;C71&amp;", "&amp;D71&amp;", '"&amp;E71&amp;"');"</f>
+        <v>INSERT INTO courses VALUES('CSCI 4325','SOFTWARE QUALITY ASSURANCE', null, null, 'BCS');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F72" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO courses VALUES('CSCI 4326','EMPIRICAL METHODS IN SOFTWARE ENGINEERING', null, null, 'BCS');</v>
       </c>

</xml_diff>